<commit_message>
dev-172 - added time parser, work_types getter and fixed spaces in tabel code
</commit_message>
<xml_diff>
--- a/etc/scripts/timetable_rows.xlsx
+++ b/etc/scripts/timetable_rows.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Расписание на подпись." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -142,7 +142,7 @@
     <t>2020-04-30</t>
   </si>
   <si>
-    <t>23739</t>
+    <t xml:space="preserve"> A23739 </t>
   </si>
   <si>
     <t>Иванов Иван Иванович</t>
@@ -185,12 +185,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,11 +204,155 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +365,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -239,9 +575,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -255,11 +833,63 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -542,27 +1172,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7083333333333" customWidth="1"/>
+    <col min="2" max="2" width="30.7083333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.7083333333333" customWidth="1"/>
+    <col min="4" max="6" width="10.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" ht="30" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" ht="30" spans="1:6">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1202,8 +1832,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="3" t="s">
+    <row r="33" ht="30" spans="1:6">
+      <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1222,7 +1852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" ht="30" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
@@ -1242,8 +1872,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
+    <row r="35" ht="30" spans="1:6">
+      <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1262,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" ht="30" spans="1:6">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1282,8 +1912,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="3" t="s">
+    <row r="37" ht="30" spans="1:6">
+      <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1302,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" ht="30" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1322,8 +1952,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3" t="s">
+    <row r="39" ht="30" spans="1:6">
+      <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1342,7 +1972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" ht="30" spans="1:6">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1362,8 +1992,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="3" t="s">
+    <row r="41" ht="30" spans="1:6">
+      <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1382,7 +2012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" ht="30" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -1402,8 +2032,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="3" t="s">
+    <row r="43" ht="30" spans="1:6">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1422,7 +2052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" ht="30" spans="1:6">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1442,8 +2072,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="3" t="s">
+    <row r="45" ht="30" spans="1:6">
+      <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -1462,7 +2092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" ht="30" spans="1:6">
       <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
@@ -1482,8 +2112,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="3" t="s">
+    <row r="47" ht="30" spans="1:6">
+      <c r="A47" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1502,7 +2132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" ht="30" spans="1:6">
       <c r="A48" s="2" t="s">
         <v>42</v>
       </c>
@@ -1522,8 +2152,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="3" t="s">
+    <row r="49" ht="30" spans="1:6">
+      <c r="A49" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -1542,7 +2172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" ht="30" spans="1:6">
       <c r="A50" s="2" t="s">
         <v>42</v>
       </c>
@@ -1562,8 +2192,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="3" t="s">
+    <row r="51" ht="30" spans="1:6">
+      <c r="A51" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1582,7 +2212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" ht="30" spans="1:6">
       <c r="A52" s="2" t="s">
         <v>42</v>
       </c>
@@ -1602,8 +2232,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="3" t="s">
+    <row r="53" ht="30" spans="1:6">
+      <c r="A53" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -1622,7 +2252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" ht="30" spans="1:6">
       <c r="A54" s="2" t="s">
         <v>42</v>
       </c>
@@ -1642,8 +2272,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="3" t="s">
+    <row r="55" ht="30" spans="1:6">
+      <c r="A55" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -1662,7 +2292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" ht="30" spans="1:6">
       <c r="A56" s="2" t="s">
         <v>42</v>
       </c>
@@ -1682,8 +2312,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="3" t="s">
+    <row r="57" ht="30" spans="1:6">
+      <c r="A57" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -1702,7 +2332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" ht="30" spans="1:6">
       <c r="A58" s="2" t="s">
         <v>42</v>
       </c>
@@ -1722,8 +2352,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="3" t="s">
+    <row r="59" ht="30" spans="1:6">
+      <c r="A59" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -1742,7 +2372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" ht="30" spans="1:6">
       <c r="A60" s="2" t="s">
         <v>42</v>
       </c>
@@ -1762,8 +2392,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="3" t="s">
+    <row r="61" ht="30" spans="1:6">
+      <c r="A61" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2382,7 +3012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" ht="30" spans="1:6">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -2402,7 +3032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" ht="30" spans="1:6">
       <c r="A93" s="3" t="s">
         <v>47</v>
       </c>
@@ -2422,7 +3052,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" ht="30" spans="1:6">
       <c r="A94" s="2" t="s">
         <v>47</v>
       </c>
@@ -2442,7 +3072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" ht="30" spans="1:6">
       <c r="A95" s="3" t="s">
         <v>47</v>
       </c>
@@ -2462,7 +3092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" ht="30" spans="1:6">
       <c r="A96" s="2" t="s">
         <v>47</v>
       </c>
@@ -2482,7 +3112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" ht="30" spans="1:6">
       <c r="A97" s="3" t="s">
         <v>47</v>
       </c>
@@ -2502,7 +3132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" ht="30" spans="1:6">
       <c r="A98" s="2" t="s">
         <v>47</v>
       </c>
@@ -2522,7 +3152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" ht="30" spans="1:6">
       <c r="A99" s="3" t="s">
         <v>47</v>
       </c>
@@ -2542,7 +3172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" ht="30" spans="1:6">
       <c r="A100" s="2" t="s">
         <v>47</v>
       </c>
@@ -2562,7 +3192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" ht="30" spans="1:6">
       <c r="A101" s="3" t="s">
         <v>47</v>
       </c>
@@ -2582,7 +3212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" ht="30" spans="1:6">
       <c r="A102" s="2" t="s">
         <v>47</v>
       </c>
@@ -2602,7 +3232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" ht="30" spans="1:6">
       <c r="A103" s="3" t="s">
         <v>47</v>
       </c>
@@ -2622,7 +3252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" ht="30" spans="1:6">
       <c r="A104" s="2" t="s">
         <v>47</v>
       </c>
@@ -2642,7 +3272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" ht="30" spans="1:6">
       <c r="A105" s="3" t="s">
         <v>47</v>
       </c>
@@ -2662,7 +3292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" ht="30" spans="1:6">
       <c r="A106" s="2" t="s">
         <v>47</v>
       </c>
@@ -2682,7 +3312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" ht="30" spans="1:6">
       <c r="A107" s="3" t="s">
         <v>47</v>
       </c>
@@ -2702,7 +3332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" ht="30" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>47</v>
       </c>
@@ -2722,7 +3352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" ht="30" spans="1:6">
       <c r="A109" s="3" t="s">
         <v>47</v>
       </c>
@@ -2742,7 +3372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" ht="30" spans="1:6">
       <c r="A110" s="2" t="s">
         <v>47</v>
       </c>
@@ -2762,7 +3392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" ht="30" spans="1:6">
       <c r="A111" s="3" t="s">
         <v>47</v>
       </c>
@@ -2782,7 +3412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" ht="30" spans="1:6">
       <c r="A112" s="2" t="s">
         <v>47</v>
       </c>
@@ -2802,7 +3432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" ht="30" spans="1:6">
       <c r="A113" s="3" t="s">
         <v>47</v>
       </c>
@@ -2822,7 +3452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" ht="30" spans="1:6">
       <c r="A114" s="2" t="s">
         <v>47</v>
       </c>
@@ -2842,7 +3472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" ht="30" spans="1:6">
       <c r="A115" s="3" t="s">
         <v>47</v>
       </c>
@@ -2862,7 +3492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" ht="30" spans="1:6">
       <c r="A116" s="2" t="s">
         <v>47</v>
       </c>
@@ -2882,7 +3512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" ht="30" spans="1:6">
       <c r="A117" s="3" t="s">
         <v>47</v>
       </c>
@@ -2902,7 +3532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" ht="30" spans="1:6">
       <c r="A118" s="2" t="s">
         <v>47</v>
       </c>
@@ -2922,7 +3552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" ht="30" spans="1:6">
       <c r="A119" s="3" t="s">
         <v>47</v>
       </c>
@@ -2942,7 +3572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" ht="30" spans="1:6">
       <c r="A120" s="2" t="s">
         <v>47</v>
       </c>
@@ -2962,7 +3592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" ht="30" spans="1:6">
       <c r="A121" s="3" t="s">
         <v>47</v>
       </c>
@@ -3582,7 +4212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" ht="30" spans="1:6">
       <c r="A152" s="2" t="s">
         <v>54</v>
       </c>
@@ -3602,7 +4232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" ht="30" spans="1:6">
       <c r="A153" s="3" t="s">
         <v>54</v>
       </c>
@@ -3622,7 +4252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" ht="30" spans="1:6">
       <c r="A154" s="2" t="s">
         <v>54</v>
       </c>
@@ -3642,7 +4272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" ht="30" spans="1:6">
       <c r="A155" s="3" t="s">
         <v>54</v>
       </c>
@@ -3662,7 +4292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" ht="30" spans="1:6">
       <c r="A156" s="2" t="s">
         <v>54</v>
       </c>
@@ -3682,7 +4312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" ht="30" spans="1:6">
       <c r="A157" s="3" t="s">
         <v>54</v>
       </c>
@@ -3702,7 +4332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" ht="30" spans="1:6">
       <c r="A158" s="2" t="s">
         <v>54</v>
       </c>
@@ -3722,7 +4352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" ht="30" spans="1:6">
       <c r="A159" s="3" t="s">
         <v>54</v>
       </c>
@@ -3742,7 +4372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" ht="30" spans="1:6">
       <c r="A160" s="2" t="s">
         <v>54</v>
       </c>
@@ -3762,7 +4392,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" ht="30" spans="1:6">
       <c r="A161" s="3" t="s">
         <v>54</v>
       </c>
@@ -3782,7 +4412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" ht="30" spans="1:6">
       <c r="A162" s="2" t="s">
         <v>54</v>
       </c>
@@ -3802,7 +4432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" ht="30" spans="1:6">
       <c r="A163" s="3" t="s">
         <v>54</v>
       </c>
@@ -3822,7 +4452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" ht="30" spans="1:6">
       <c r="A164" s="2" t="s">
         <v>54</v>
       </c>
@@ -3842,7 +4472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" ht="30" spans="1:6">
       <c r="A165" s="3" t="s">
         <v>54</v>
       </c>
@@ -3862,7 +4492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" ht="30" spans="1:6">
       <c r="A166" s="2" t="s">
         <v>54</v>
       </c>
@@ -3882,7 +4512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" ht="30" spans="1:6">
       <c r="A167" s="3" t="s">
         <v>54</v>
       </c>
@@ -3902,7 +4532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" ht="30" spans="1:6">
       <c r="A168" s="2" t="s">
         <v>54</v>
       </c>
@@ -3922,7 +4552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" ht="30" spans="1:6">
       <c r="A169" s="3" t="s">
         <v>54</v>
       </c>
@@ -3942,7 +4572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" ht="30" spans="1:6">
       <c r="A170" s="2" t="s">
         <v>54</v>
       </c>
@@ -3962,7 +4592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" ht="30" spans="1:6">
       <c r="A171" s="3" t="s">
         <v>54</v>
       </c>
@@ -3982,7 +4612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" ht="30" spans="1:6">
       <c r="A172" s="2" t="s">
         <v>54</v>
       </c>
@@ -4002,7 +4632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" ht="30" spans="1:6">
       <c r="A173" s="3" t="s">
         <v>54</v>
       </c>
@@ -4022,7 +4652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" ht="30" spans="1:6">
       <c r="A174" s="2" t="s">
         <v>54</v>
       </c>
@@ -4042,7 +4672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" ht="30" spans="1:6">
       <c r="A175" s="3" t="s">
         <v>54</v>
       </c>
@@ -4062,7 +4692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" ht="30" spans="1:6">
       <c r="A176" s="2" t="s">
         <v>54</v>
       </c>
@@ -4082,7 +4712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" ht="30" spans="1:6">
       <c r="A177" s="3" t="s">
         <v>54</v>
       </c>
@@ -4102,7 +4732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" ht="30" spans="1:6">
       <c r="A178" s="2" t="s">
         <v>54</v>
       </c>
@@ -4122,7 +4752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" ht="30" spans="1:6">
       <c r="A179" s="3" t="s">
         <v>54</v>
       </c>
@@ -4142,7 +4772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" ht="30" spans="1:6">
       <c r="A180" s="2" t="s">
         <v>54</v>
       </c>
@@ -4162,7 +4792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" ht="30" spans="1:6">
       <c r="A181" s="3" t="s">
         <v>54</v>
       </c>
@@ -4184,5 +4814,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>